<commit_message>
update movement in group file, fix recruitment option in biol file, update recruit time in spreadsheet
</commit_message>
<xml_diff>
--- a/R/BHrecruits.xlsx
+++ b/R/BHrecruits.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="554" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BH" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="1082">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="1082">
   <si>
     <t>BHalpha_ANC</t>
   </si>
@@ -3319,7 +3319,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3632,7 +3662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
@@ -6790,10 +6820,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R64"/>
+  <dimension ref="A1:S129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="Q79" sqref="Q79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6806,7 +6836,7 @@
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
@@ -8629,7 +8659,7 @@
         <v>1</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="3">B34*D34</f>
+        <f t="shared" ref="E34:E60" si="3">B34*D34</f>
         <v>2</v>
       </c>
       <c r="F34" t="s">
@@ -10263,9 +10293,2957 @@
         <v>367</v>
       </c>
     </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>267</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E125" si="4">B67*D67</f>
+        <v>2</v>
+      </c>
+      <c r="F67" t="s">
+        <v>269</v>
+      </c>
+      <c r="G67">
+        <v>210</v>
+      </c>
+      <c r="H67" t="s">
+        <v>270</v>
+      </c>
+      <c r="I67">
+        <v>7</v>
+      </c>
+      <c r="J67" t="s">
+        <v>271</v>
+      </c>
+      <c r="K67">
+        <v>30</v>
+      </c>
+      <c r="L67" t="s">
+        <v>272</v>
+      </c>
+      <c r="M67">
+        <v>60</v>
+      </c>
+      <c r="N67" t="s">
+        <v>392</v>
+      </c>
+      <c r="O67">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>274</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>275</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F68" t="s">
+        <v>276</v>
+      </c>
+      <c r="G68">
+        <v>290</v>
+      </c>
+      <c r="H68" t="s">
+        <v>277</v>
+      </c>
+      <c r="I68">
+        <v>7</v>
+      </c>
+      <c r="J68" t="s">
+        <v>278</v>
+      </c>
+      <c r="K68">
+        <v>30</v>
+      </c>
+      <c r="L68" t="s">
+        <v>279</v>
+      </c>
+      <c r="M68">
+        <v>60</v>
+      </c>
+      <c r="N68" t="s">
+        <v>357</v>
+      </c>
+      <c r="O68">
+        <v>27900.25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>281</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>282</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F69" t="s">
+        <v>283</v>
+      </c>
+      <c r="G69">
+        <v>180</v>
+      </c>
+      <c r="H69" t="s">
+        <v>284</v>
+      </c>
+      <c r="I69">
+        <v>7</v>
+      </c>
+      <c r="J69" t="s">
+        <v>285</v>
+      </c>
+      <c r="K69">
+        <v>60</v>
+      </c>
+      <c r="L69" t="s">
+        <v>286</v>
+      </c>
+      <c r="M69">
+        <v>90</v>
+      </c>
+      <c r="N69" t="s">
+        <v>371</v>
+      </c>
+      <c r="O69">
+        <v>21083.35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>288</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>289</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
+        <v>290</v>
+      </c>
+      <c r="G70">
+        <v>180</v>
+      </c>
+      <c r="H70" t="s">
+        <v>291</v>
+      </c>
+      <c r="I70">
+        <v>7</v>
+      </c>
+      <c r="J70" t="s">
+        <v>292</v>
+      </c>
+      <c r="K70">
+        <v>30</v>
+      </c>
+      <c r="L70" t="s">
+        <v>293</v>
+      </c>
+      <c r="M70">
+        <v>30</v>
+      </c>
+      <c r="N70" t="s">
+        <v>294</v>
+      </c>
+      <c r="O70">
+        <v>99.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>295</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>296</v>
+      </c>
+      <c r="D71">
+        <v>3</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F71" t="s">
+        <v>297</v>
+      </c>
+      <c r="G71">
+        <v>180</v>
+      </c>
+      <c r="H71" t="s">
+        <v>298</v>
+      </c>
+      <c r="I71">
+        <v>7</v>
+      </c>
+      <c r="J71" t="s">
+        <v>299</v>
+      </c>
+      <c r="K71">
+        <v>80</v>
+      </c>
+      <c r="L71" t="s">
+        <v>300</v>
+      </c>
+      <c r="M71">
+        <v>90</v>
+      </c>
+      <c r="N71" t="s">
+        <v>588</v>
+      </c>
+      <c r="O71">
+        <v>5678.88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>302</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
+        <v>303</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F72" t="s">
+        <v>304</v>
+      </c>
+      <c r="G72">
+        <v>270</v>
+      </c>
+      <c r="H72" t="s">
+        <v>305</v>
+      </c>
+      <c r="I72">
+        <v>7</v>
+      </c>
+      <c r="J72" t="s">
+        <v>306</v>
+      </c>
+      <c r="K72">
+        <v>80</v>
+      </c>
+      <c r="L72" t="s">
+        <v>307</v>
+      </c>
+      <c r="M72">
+        <v>90</v>
+      </c>
+      <c r="N72" t="s">
+        <v>399</v>
+      </c>
+      <c r="O72">
+        <v>17.809999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>309</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
+        <v>310</v>
+      </c>
+      <c r="D73">
+        <v>3</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F73" t="s">
+        <v>311</v>
+      </c>
+      <c r="G73">
+        <v>30</v>
+      </c>
+      <c r="H73" t="s">
+        <v>312</v>
+      </c>
+      <c r="I73">
+        <v>7</v>
+      </c>
+      <c r="J73" t="s">
+        <v>313</v>
+      </c>
+      <c r="K73">
+        <v>80</v>
+      </c>
+      <c r="L73" t="s">
+        <v>314</v>
+      </c>
+      <c r="M73">
+        <v>90</v>
+      </c>
+      <c r="N73" t="s">
+        <v>462</v>
+      </c>
+      <c r="O73">
+        <v>134.86000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>316</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+      <c r="C74" t="s">
+        <v>317</v>
+      </c>
+      <c r="D74">
+        <v>3</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F74" t="s">
+        <v>318</v>
+      </c>
+      <c r="G74">
+        <v>100</v>
+      </c>
+      <c r="H74" t="s">
+        <v>319</v>
+      </c>
+      <c r="I74">
+        <v>7</v>
+      </c>
+      <c r="J74" t="s">
+        <v>320</v>
+      </c>
+      <c r="K74">
+        <v>120</v>
+      </c>
+      <c r="L74" t="s">
+        <v>321</v>
+      </c>
+      <c r="M74">
+        <v>90</v>
+      </c>
+      <c r="N74" t="s">
+        <v>385</v>
+      </c>
+      <c r="O74">
+        <v>11.95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>323</v>
+      </c>
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75" t="s">
+        <v>324</v>
+      </c>
+      <c r="D75">
+        <v>3</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F75" t="s">
+        <v>325</v>
+      </c>
+      <c r="G75">
+        <v>180</v>
+      </c>
+      <c r="H75" t="s">
+        <v>326</v>
+      </c>
+      <c r="I75">
+        <v>7</v>
+      </c>
+      <c r="J75" t="s">
+        <v>327</v>
+      </c>
+      <c r="K75">
+        <v>80</v>
+      </c>
+      <c r="L75" t="s">
+        <v>328</v>
+      </c>
+      <c r="M75">
+        <v>90</v>
+      </c>
+      <c r="N75" t="s">
+        <v>658</v>
+      </c>
+      <c r="O75">
+        <v>3525480.78</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>330</v>
+      </c>
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76" t="s">
+        <v>331</v>
+      </c>
+      <c r="D76">
+        <v>3</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F76" t="s">
+        <v>332</v>
+      </c>
+      <c r="G76">
+        <v>100</v>
+      </c>
+      <c r="H76" t="s">
+        <v>333</v>
+      </c>
+      <c r="I76">
+        <v>7</v>
+      </c>
+      <c r="J76" t="s">
+        <v>334</v>
+      </c>
+      <c r="K76">
+        <v>80</v>
+      </c>
+      <c r="L76" t="s">
+        <v>335</v>
+      </c>
+      <c r="M76">
+        <v>90</v>
+      </c>
+      <c r="N76" t="s">
+        <v>427</v>
+      </c>
+      <c r="O76">
+        <v>763.46</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>337</v>
+      </c>
+      <c r="B77">
+        <v>2</v>
+      </c>
+      <c r="C77" t="s">
+        <v>338</v>
+      </c>
+      <c r="D77">
+        <v>3</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F77" t="s">
+        <v>339</v>
+      </c>
+      <c r="G77">
+        <v>180</v>
+      </c>
+      <c r="H77" t="s">
+        <v>340</v>
+      </c>
+      <c r="I77">
+        <v>7</v>
+      </c>
+      <c r="J77" t="s">
+        <v>341</v>
+      </c>
+      <c r="K77">
+        <v>80</v>
+      </c>
+      <c r="L77" t="s">
+        <v>342</v>
+      </c>
+      <c r="M77">
+        <v>90</v>
+      </c>
+      <c r="N77" t="s">
+        <v>560</v>
+      </c>
+      <c r="O77">
+        <v>795.66</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>344</v>
+      </c>
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78" t="s">
+        <v>345</v>
+      </c>
+      <c r="D78">
+        <v>3</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F78" t="s">
+        <v>346</v>
+      </c>
+      <c r="G78">
+        <v>180</v>
+      </c>
+      <c r="H78" t="s">
+        <v>347</v>
+      </c>
+      <c r="I78">
+        <v>7</v>
+      </c>
+      <c r="J78" t="s">
+        <v>348</v>
+      </c>
+      <c r="K78">
+        <v>80</v>
+      </c>
+      <c r="L78" t="s">
+        <v>349</v>
+      </c>
+      <c r="M78">
+        <v>90</v>
+      </c>
+      <c r="N78" t="s">
+        <v>504</v>
+      </c>
+      <c r="O78">
+        <v>95.78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>351</v>
+      </c>
+      <c r="B79">
+        <v>3</v>
+      </c>
+      <c r="C79" t="s">
+        <v>352</v>
+      </c>
+      <c r="D79">
+        <v>3</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="F79" t="s">
+        <v>353</v>
+      </c>
+      <c r="G79">
+        <v>180</v>
+      </c>
+      <c r="H79" t="s">
+        <v>354</v>
+      </c>
+      <c r="I79">
+        <v>7</v>
+      </c>
+      <c r="J79" t="s">
+        <v>355</v>
+      </c>
+      <c r="K79">
+        <v>180</v>
+      </c>
+      <c r="L79" t="s">
+        <v>356</v>
+      </c>
+      <c r="M79">
+        <v>60</v>
+      </c>
+      <c r="N79" t="s">
+        <v>581</v>
+      </c>
+      <c r="O79">
+        <v>21317.17</v>
+      </c>
+      <c r="Q79">
+        <f>G79+K79+I79</f>
+        <v>367</v>
+      </c>
+      <c r="R79">
+        <f>Q79+M79</f>
+        <v>427</v>
+      </c>
+      <c r="S79">
+        <f>R79-365-I79</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>358</v>
+      </c>
+      <c r="B80">
+        <v>3</v>
+      </c>
+      <c r="C80" t="s">
+        <v>359</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="F80" t="s">
+        <v>360</v>
+      </c>
+      <c r="G80">
+        <v>180</v>
+      </c>
+      <c r="H80" t="s">
+        <v>361</v>
+      </c>
+      <c r="I80">
+        <v>7</v>
+      </c>
+      <c r="J80" t="s">
+        <v>362</v>
+      </c>
+      <c r="K80">
+        <v>180</v>
+      </c>
+      <c r="L80" t="s">
+        <v>363</v>
+      </c>
+      <c r="M80">
+        <v>60</v>
+      </c>
+      <c r="N80" t="s">
+        <v>420</v>
+      </c>
+      <c r="O80">
+        <v>82.43</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>365</v>
+      </c>
+      <c r="B81">
+        <v>3</v>
+      </c>
+      <c r="C81" t="s">
+        <v>366</v>
+      </c>
+      <c r="D81">
+        <v>3</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="F81" t="s">
+        <v>367</v>
+      </c>
+      <c r="G81">
+        <v>180</v>
+      </c>
+      <c r="H81" t="s">
+        <v>368</v>
+      </c>
+      <c r="I81">
+        <v>7</v>
+      </c>
+      <c r="J81" t="s">
+        <v>369</v>
+      </c>
+      <c r="K81">
+        <v>180</v>
+      </c>
+      <c r="L81" t="s">
+        <v>370</v>
+      </c>
+      <c r="M81">
+        <v>60</v>
+      </c>
+      <c r="N81" t="s">
+        <v>539</v>
+      </c>
+      <c r="O81">
+        <v>54.03</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>372</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>373</v>
+      </c>
+      <c r="D82">
+        <v>2</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F82" t="s">
+        <v>374</v>
+      </c>
+      <c r="G82">
+        <v>180</v>
+      </c>
+      <c r="H82" t="s">
+        <v>375</v>
+      </c>
+      <c r="I82">
+        <v>7</v>
+      </c>
+      <c r="J82" t="s">
+        <v>376</v>
+      </c>
+      <c r="K82">
+        <v>25</v>
+      </c>
+      <c r="L82" t="s">
+        <v>377</v>
+      </c>
+      <c r="M82">
+        <v>30</v>
+      </c>
+      <c r="N82" t="s">
+        <v>350</v>
+      </c>
+      <c r="O82">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>379</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>380</v>
+      </c>
+      <c r="D83">
+        <v>3</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F83" t="s">
+        <v>381</v>
+      </c>
+      <c r="G83">
+        <v>100</v>
+      </c>
+      <c r="H83" t="s">
+        <v>382</v>
+      </c>
+      <c r="I83">
+        <v>7</v>
+      </c>
+      <c r="J83" t="s">
+        <v>383</v>
+      </c>
+      <c r="K83">
+        <v>35</v>
+      </c>
+      <c r="L83" t="s">
+        <v>384</v>
+      </c>
+      <c r="M83">
+        <v>40</v>
+      </c>
+      <c r="N83" t="s">
+        <v>343</v>
+      </c>
+      <c r="O83">
+        <v>24.13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>386</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>387</v>
+      </c>
+      <c r="D84">
+        <v>3</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F84" t="s">
+        <v>388</v>
+      </c>
+      <c r="G84">
+        <v>100</v>
+      </c>
+      <c r="H84" t="s">
+        <v>389</v>
+      </c>
+      <c r="I84">
+        <v>7</v>
+      </c>
+      <c r="J84" t="s">
+        <v>390</v>
+      </c>
+      <c r="K84">
+        <v>35</v>
+      </c>
+      <c r="L84" t="s">
+        <v>391</v>
+      </c>
+      <c r="M84">
+        <v>40</v>
+      </c>
+      <c r="N84" t="s">
+        <v>406</v>
+      </c>
+      <c r="O84">
+        <v>154.37</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>393</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
+        <v>394</v>
+      </c>
+      <c r="D85">
+        <v>3</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F85" t="s">
+        <v>395</v>
+      </c>
+      <c r="G85">
+        <v>100</v>
+      </c>
+      <c r="H85" t="s">
+        <v>396</v>
+      </c>
+      <c r="I85">
+        <v>7</v>
+      </c>
+      <c r="J85" t="s">
+        <v>397</v>
+      </c>
+      <c r="K85">
+        <v>35</v>
+      </c>
+      <c r="L85" t="s">
+        <v>398</v>
+      </c>
+      <c r="M85">
+        <v>40</v>
+      </c>
+      <c r="N85" t="s">
+        <v>546</v>
+      </c>
+      <c r="O85">
+        <v>143.11000000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>400</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86" t="s">
+        <v>401</v>
+      </c>
+      <c r="D86">
+        <v>3</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F86" t="s">
+        <v>402</v>
+      </c>
+      <c r="G86">
+        <v>280</v>
+      </c>
+      <c r="H86" t="s">
+        <v>403</v>
+      </c>
+      <c r="I86">
+        <v>7</v>
+      </c>
+      <c r="J86" t="s">
+        <v>404</v>
+      </c>
+      <c r="K86">
+        <v>60</v>
+      </c>
+      <c r="L86" t="s">
+        <v>405</v>
+      </c>
+      <c r="M86">
+        <v>60</v>
+      </c>
+      <c r="N86" t="s">
+        <v>329</v>
+      </c>
+      <c r="O86">
+        <v>3825.02</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>407</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87" t="s">
+        <v>408</v>
+      </c>
+      <c r="D87">
+        <v>2</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F87" t="s">
+        <v>409</v>
+      </c>
+      <c r="G87">
+        <v>270</v>
+      </c>
+      <c r="H87" t="s">
+        <v>410</v>
+      </c>
+      <c r="I87">
+        <v>7</v>
+      </c>
+      <c r="J87" t="s">
+        <v>411</v>
+      </c>
+      <c r="K87">
+        <v>30</v>
+      </c>
+      <c r="L87" t="s">
+        <v>412</v>
+      </c>
+      <c r="M87">
+        <v>40</v>
+      </c>
+      <c r="N87" t="s">
+        <v>280</v>
+      </c>
+      <c r="O87">
+        <v>13.34</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>414</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88" t="s">
+        <v>415</v>
+      </c>
+      <c r="D88">
+        <v>2</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F88" t="s">
+        <v>416</v>
+      </c>
+      <c r="G88">
+        <v>10</v>
+      </c>
+      <c r="H88" t="s">
+        <v>417</v>
+      </c>
+      <c r="I88">
+        <v>7</v>
+      </c>
+      <c r="J88" t="s">
+        <v>418</v>
+      </c>
+      <c r="K88">
+        <v>30</v>
+      </c>
+      <c r="L88" t="s">
+        <v>419</v>
+      </c>
+      <c r="M88">
+        <v>40</v>
+      </c>
+      <c r="N88" t="s">
+        <v>679</v>
+      </c>
+      <c r="O88">
+        <v>82.92</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>421</v>
+      </c>
+      <c r="B89">
+        <v>2</v>
+      </c>
+      <c r="C89" t="s">
+        <v>422</v>
+      </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F89" t="s">
+        <v>423</v>
+      </c>
+      <c r="G89">
+        <v>20</v>
+      </c>
+      <c r="H89" t="s">
+        <v>424</v>
+      </c>
+      <c r="I89">
+        <v>7</v>
+      </c>
+      <c r="J89" t="s">
+        <v>425</v>
+      </c>
+      <c r="K89">
+        <v>60</v>
+      </c>
+      <c r="L89" t="s">
+        <v>426</v>
+      </c>
+      <c r="M89">
+        <v>90</v>
+      </c>
+      <c r="N89" t="s">
+        <v>616</v>
+      </c>
+      <c r="O89">
+        <v>207.63</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>428</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="C90" t="s">
+        <v>429</v>
+      </c>
+      <c r="D90">
+        <v>3</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F90" t="s">
+        <v>430</v>
+      </c>
+      <c r="G90">
+        <v>150</v>
+      </c>
+      <c r="H90" t="s">
+        <v>431</v>
+      </c>
+      <c r="I90">
+        <v>7</v>
+      </c>
+      <c r="J90" t="s">
+        <v>432</v>
+      </c>
+      <c r="K90">
+        <v>30</v>
+      </c>
+      <c r="L90" t="s">
+        <v>433</v>
+      </c>
+      <c r="M90">
+        <v>90</v>
+      </c>
+      <c r="N90" t="s">
+        <v>273</v>
+      </c>
+      <c r="O90">
+        <v>18.11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>435</v>
+      </c>
+      <c r="B91">
+        <v>2</v>
+      </c>
+      <c r="C91" t="s">
+        <v>436</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F91" t="s">
+        <v>437</v>
+      </c>
+      <c r="G91">
+        <v>150</v>
+      </c>
+      <c r="H91" t="s">
+        <v>438</v>
+      </c>
+      <c r="I91">
+        <v>7</v>
+      </c>
+      <c r="J91" t="s">
+        <v>439</v>
+      </c>
+      <c r="K91">
+        <v>30</v>
+      </c>
+      <c r="L91" t="s">
+        <v>440</v>
+      </c>
+      <c r="M91">
+        <v>90</v>
+      </c>
+      <c r="N91" t="s">
+        <v>413</v>
+      </c>
+      <c r="O91">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>442</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="C92" t="s">
+        <v>443</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F92" t="s">
+        <v>444</v>
+      </c>
+      <c r="G92">
+        <v>10</v>
+      </c>
+      <c r="H92" t="s">
+        <v>445</v>
+      </c>
+      <c r="I92">
+        <v>7</v>
+      </c>
+      <c r="J92" t="s">
+        <v>446</v>
+      </c>
+      <c r="K92">
+        <v>30</v>
+      </c>
+      <c r="L92" t="s">
+        <v>447</v>
+      </c>
+      <c r="M92">
+        <v>90</v>
+      </c>
+      <c r="N92" t="s">
+        <v>378</v>
+      </c>
+      <c r="O92">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>449</v>
+      </c>
+      <c r="B93">
+        <v>2</v>
+      </c>
+      <c r="C93" t="s">
+        <v>450</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F93" t="s">
+        <v>451</v>
+      </c>
+      <c r="G93">
+        <v>180</v>
+      </c>
+      <c r="H93" t="s">
+        <v>452</v>
+      </c>
+      <c r="I93">
+        <v>7</v>
+      </c>
+      <c r="J93" t="s">
+        <v>453</v>
+      </c>
+      <c r="K93">
+        <v>30</v>
+      </c>
+      <c r="L93" t="s">
+        <v>454</v>
+      </c>
+      <c r="M93">
+        <v>90</v>
+      </c>
+      <c r="N93" t="s">
+        <v>441</v>
+      </c>
+      <c r="O93">
+        <v>32.65</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>456</v>
+      </c>
+      <c r="B94">
+        <v>2</v>
+      </c>
+      <c r="C94" t="s">
+        <v>457</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F94" t="s">
+        <v>458</v>
+      </c>
+      <c r="G94">
+        <v>150</v>
+      </c>
+      <c r="H94" t="s">
+        <v>459</v>
+      </c>
+      <c r="I94">
+        <v>7</v>
+      </c>
+      <c r="J94" t="s">
+        <v>460</v>
+      </c>
+      <c r="K94">
+        <v>30</v>
+      </c>
+      <c r="L94" t="s">
+        <v>461</v>
+      </c>
+      <c r="M94">
+        <v>90</v>
+      </c>
+      <c r="N94" t="s">
+        <v>490</v>
+      </c>
+      <c r="O94">
+        <v>127.1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>463</v>
+      </c>
+      <c r="B95">
+        <v>2</v>
+      </c>
+      <c r="C95" t="s">
+        <v>464</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F95" t="s">
+        <v>465</v>
+      </c>
+      <c r="G95">
+        <v>150</v>
+      </c>
+      <c r="H95" t="s">
+        <v>466</v>
+      </c>
+      <c r="I95">
+        <v>7</v>
+      </c>
+      <c r="J95" t="s">
+        <v>467</v>
+      </c>
+      <c r="K95">
+        <v>30</v>
+      </c>
+      <c r="L95" t="s">
+        <v>468</v>
+      </c>
+      <c r="M95">
+        <v>90</v>
+      </c>
+      <c r="N95" t="s">
+        <v>637</v>
+      </c>
+      <c r="O95">
+        <v>11810.41</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>470</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+      <c r="C96" t="s">
+        <v>471</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F96" t="s">
+        <v>472</v>
+      </c>
+      <c r="G96">
+        <v>150</v>
+      </c>
+      <c r="H96" t="s">
+        <v>473</v>
+      </c>
+      <c r="I96">
+        <v>7</v>
+      </c>
+      <c r="J96" t="s">
+        <v>474</v>
+      </c>
+      <c r="K96">
+        <v>30</v>
+      </c>
+      <c r="L96" t="s">
+        <v>475</v>
+      </c>
+      <c r="M96">
+        <v>90</v>
+      </c>
+      <c r="N96" t="s">
+        <v>336</v>
+      </c>
+      <c r="O96">
+        <v>77.02</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>477</v>
+      </c>
+      <c r="B97">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
+        <v>478</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F97" t="s">
+        <v>479</v>
+      </c>
+      <c r="G97">
+        <v>100</v>
+      </c>
+      <c r="H97" t="s">
+        <v>480</v>
+      </c>
+      <c r="I97">
+        <v>7</v>
+      </c>
+      <c r="J97" t="s">
+        <v>481</v>
+      </c>
+      <c r="K97">
+        <v>30</v>
+      </c>
+      <c r="L97" t="s">
+        <v>482</v>
+      </c>
+      <c r="M97">
+        <v>90</v>
+      </c>
+      <c r="N97" t="s">
+        <v>448</v>
+      </c>
+      <c r="O97">
+        <v>621.19000000000005</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>484</v>
+      </c>
+      <c r="B98">
+        <v>2</v>
+      </c>
+      <c r="C98" t="s">
+        <v>485</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F98" t="s">
+        <v>486</v>
+      </c>
+      <c r="G98">
+        <v>100</v>
+      </c>
+      <c r="H98" t="s">
+        <v>487</v>
+      </c>
+      <c r="I98">
+        <v>7</v>
+      </c>
+      <c r="J98" t="s">
+        <v>488</v>
+      </c>
+      <c r="K98">
+        <v>30</v>
+      </c>
+      <c r="L98" t="s">
+        <v>489</v>
+      </c>
+      <c r="M98">
+        <v>90</v>
+      </c>
+      <c r="N98" t="s">
+        <v>595</v>
+      </c>
+      <c r="O98">
+        <v>7165.5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>491</v>
+      </c>
+      <c r="B99">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s">
+        <v>492</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F99" t="s">
+        <v>493</v>
+      </c>
+      <c r="G99">
+        <v>220</v>
+      </c>
+      <c r="H99" t="s">
+        <v>494</v>
+      </c>
+      <c r="I99">
+        <v>7</v>
+      </c>
+      <c r="J99" t="s">
+        <v>495</v>
+      </c>
+      <c r="K99">
+        <v>30</v>
+      </c>
+      <c r="L99" t="s">
+        <v>496</v>
+      </c>
+      <c r="M99">
+        <v>90</v>
+      </c>
+      <c r="N99" t="s">
+        <v>602</v>
+      </c>
+      <c r="O99">
+        <v>21158.53</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>498</v>
+      </c>
+      <c r="B100">
+        <v>2</v>
+      </c>
+      <c r="C100" t="s">
+        <v>499</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F100" t="s">
+        <v>500</v>
+      </c>
+      <c r="G100">
+        <v>180</v>
+      </c>
+      <c r="H100" t="s">
+        <v>501</v>
+      </c>
+      <c r="I100">
+        <v>7</v>
+      </c>
+      <c r="J100" t="s">
+        <v>502</v>
+      </c>
+      <c r="K100">
+        <v>30</v>
+      </c>
+      <c r="L100" t="s">
+        <v>503</v>
+      </c>
+      <c r="M100">
+        <v>90</v>
+      </c>
+      <c r="N100" t="s">
+        <v>483</v>
+      </c>
+      <c r="O100">
+        <v>8.73</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>505</v>
+      </c>
+      <c r="B101">
+        <v>2</v>
+      </c>
+      <c r="C101" t="s">
+        <v>506</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F101" t="s">
+        <v>507</v>
+      </c>
+      <c r="G101">
+        <v>180</v>
+      </c>
+      <c r="H101" t="s">
+        <v>508</v>
+      </c>
+      <c r="I101">
+        <v>7</v>
+      </c>
+      <c r="J101" t="s">
+        <v>509</v>
+      </c>
+      <c r="K101">
+        <v>30</v>
+      </c>
+      <c r="L101" t="s">
+        <v>510</v>
+      </c>
+      <c r="M101">
+        <v>90</v>
+      </c>
+      <c r="N101" t="s">
+        <v>644</v>
+      </c>
+      <c r="O101">
+        <v>12248.15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>512</v>
+      </c>
+      <c r="B102">
+        <v>2</v>
+      </c>
+      <c r="C102" t="s">
+        <v>513</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F102" t="s">
+        <v>514</v>
+      </c>
+      <c r="G102">
+        <v>180</v>
+      </c>
+      <c r="H102" t="s">
+        <v>515</v>
+      </c>
+      <c r="I102">
+        <v>7</v>
+      </c>
+      <c r="J102" t="s">
+        <v>516</v>
+      </c>
+      <c r="K102">
+        <v>30</v>
+      </c>
+      <c r="L102" t="s">
+        <v>517</v>
+      </c>
+      <c r="M102">
+        <v>90</v>
+      </c>
+      <c r="N102" t="s">
+        <v>455</v>
+      </c>
+      <c r="O102">
+        <v>111.1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>519</v>
+      </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103" t="s">
+        <v>520</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F103" t="s">
+        <v>521</v>
+      </c>
+      <c r="G103">
+        <v>10</v>
+      </c>
+      <c r="H103" t="s">
+        <v>522</v>
+      </c>
+      <c r="I103">
+        <v>7</v>
+      </c>
+      <c r="J103" t="s">
+        <v>523</v>
+      </c>
+      <c r="K103">
+        <v>30</v>
+      </c>
+      <c r="L103" t="s">
+        <v>524</v>
+      </c>
+      <c r="M103">
+        <v>90</v>
+      </c>
+      <c r="N103" t="s">
+        <v>651</v>
+      </c>
+      <c r="O103">
+        <v>4310573.47</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>526</v>
+      </c>
+      <c r="B104">
+        <v>2</v>
+      </c>
+      <c r="C104" t="s">
+        <v>527</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F104" t="s">
+        <v>528</v>
+      </c>
+      <c r="G104">
+        <v>10</v>
+      </c>
+      <c r="H104" t="s">
+        <v>529</v>
+      </c>
+      <c r="I104">
+        <v>7</v>
+      </c>
+      <c r="J104" t="s">
+        <v>530</v>
+      </c>
+      <c r="K104">
+        <v>30</v>
+      </c>
+      <c r="L104" t="s">
+        <v>531</v>
+      </c>
+      <c r="M104">
+        <v>90</v>
+      </c>
+      <c r="N104" t="s">
+        <v>497</v>
+      </c>
+      <c r="O104">
+        <v>1035.6400000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>533</v>
+      </c>
+      <c r="B105">
+        <v>2</v>
+      </c>
+      <c r="C105" t="s">
+        <v>534</v>
+      </c>
+      <c r="D105">
+        <v>1</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F105" t="s">
+        <v>535</v>
+      </c>
+      <c r="G105">
+        <v>10</v>
+      </c>
+      <c r="H105" t="s">
+        <v>536</v>
+      </c>
+      <c r="I105">
+        <v>7</v>
+      </c>
+      <c r="J105" t="s">
+        <v>537</v>
+      </c>
+      <c r="K105">
+        <v>30</v>
+      </c>
+      <c r="L105" t="s">
+        <v>538</v>
+      </c>
+      <c r="M105">
+        <v>90</v>
+      </c>
+      <c r="N105" t="s">
+        <v>630</v>
+      </c>
+      <c r="O105">
+        <v>54.32</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>540</v>
+      </c>
+      <c r="B106">
+        <v>2</v>
+      </c>
+      <c r="C106" t="s">
+        <v>541</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F106" t="s">
+        <v>542</v>
+      </c>
+      <c r="G106">
+        <v>30</v>
+      </c>
+      <c r="H106" t="s">
+        <v>543</v>
+      </c>
+      <c r="I106">
+        <v>7</v>
+      </c>
+      <c r="J106" t="s">
+        <v>544</v>
+      </c>
+      <c r="K106">
+        <v>30</v>
+      </c>
+      <c r="L106" t="s">
+        <v>545</v>
+      </c>
+      <c r="M106">
+        <v>90</v>
+      </c>
+      <c r="N106" t="s">
+        <v>469</v>
+      </c>
+      <c r="O106">
+        <v>56.67</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>547</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107" t="s">
+        <v>548</v>
+      </c>
+      <c r="D107">
+        <v>2</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F107" t="s">
+        <v>549</v>
+      </c>
+      <c r="G107">
+        <v>60</v>
+      </c>
+      <c r="H107" t="s">
+        <v>550</v>
+      </c>
+      <c r="I107">
+        <v>7</v>
+      </c>
+      <c r="J107" t="s">
+        <v>551</v>
+      </c>
+      <c r="K107">
+        <v>40</v>
+      </c>
+      <c r="L107" t="s">
+        <v>552</v>
+      </c>
+      <c r="M107">
+        <v>90</v>
+      </c>
+      <c r="N107" t="s">
+        <v>532</v>
+      </c>
+      <c r="O107">
+        <v>476.74</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>554</v>
+      </c>
+      <c r="B108">
+        <v>4</v>
+      </c>
+      <c r="C108" t="s">
+        <v>555</v>
+      </c>
+      <c r="D108">
+        <v>3</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="F108" t="s">
+        <v>556</v>
+      </c>
+      <c r="G108">
+        <v>180</v>
+      </c>
+      <c r="H108" t="s">
+        <v>557</v>
+      </c>
+      <c r="I108">
+        <v>7</v>
+      </c>
+      <c r="J108" t="s">
+        <v>558</v>
+      </c>
+      <c r="K108">
+        <v>270</v>
+      </c>
+      <c r="L108" t="s">
+        <v>559</v>
+      </c>
+      <c r="M108">
+        <v>90</v>
+      </c>
+      <c r="N108" t="s">
+        <v>434</v>
+      </c>
+      <c r="O108">
+        <v>23.28</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>561</v>
+      </c>
+      <c r="B109">
+        <v>5</v>
+      </c>
+      <c r="C109" t="s">
+        <v>562</v>
+      </c>
+      <c r="D109">
+        <v>2</v>
+      </c>
+      <c r="E109">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="F109" t="s">
+        <v>563</v>
+      </c>
+      <c r="G109">
+        <v>160</v>
+      </c>
+      <c r="H109" t="s">
+        <v>564</v>
+      </c>
+      <c r="I109">
+        <v>7</v>
+      </c>
+      <c r="J109" t="s">
+        <v>565</v>
+      </c>
+      <c r="K109">
+        <v>360</v>
+      </c>
+      <c r="L109" t="s">
+        <v>566</v>
+      </c>
+      <c r="M109">
+        <v>90</v>
+      </c>
+      <c r="N109" t="s">
+        <v>623</v>
+      </c>
+      <c r="O109">
+        <v>1201.82</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>568</v>
+      </c>
+      <c r="B110">
+        <v>5</v>
+      </c>
+      <c r="C110" t="s">
+        <v>569</v>
+      </c>
+      <c r="D110">
+        <v>2</v>
+      </c>
+      <c r="E110">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="F110" t="s">
+        <v>570</v>
+      </c>
+      <c r="G110">
+        <v>160</v>
+      </c>
+      <c r="H110" t="s">
+        <v>571</v>
+      </c>
+      <c r="I110">
+        <v>7</v>
+      </c>
+      <c r="J110" t="s">
+        <v>572</v>
+      </c>
+      <c r="K110">
+        <v>360</v>
+      </c>
+      <c r="L110" t="s">
+        <v>573</v>
+      </c>
+      <c r="M110">
+        <v>90</v>
+      </c>
+      <c r="N110" t="s">
+        <v>567</v>
+      </c>
+      <c r="O110">
+        <v>436.41</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>575</v>
+      </c>
+      <c r="B111">
+        <v>5</v>
+      </c>
+      <c r="C111" t="s">
+        <v>576</v>
+      </c>
+      <c r="D111">
+        <v>2</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="F111" t="s">
+        <v>577</v>
+      </c>
+      <c r="G111">
+        <v>160</v>
+      </c>
+      <c r="H111" t="s">
+        <v>578</v>
+      </c>
+      <c r="I111">
+        <v>7</v>
+      </c>
+      <c r="J111" t="s">
+        <v>579</v>
+      </c>
+      <c r="K111">
+        <v>360</v>
+      </c>
+      <c r="L111" t="s">
+        <v>580</v>
+      </c>
+      <c r="M111">
+        <v>90</v>
+      </c>
+      <c r="N111" t="s">
+        <v>574</v>
+      </c>
+      <c r="O111">
+        <v>3884.39</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>582</v>
+      </c>
+      <c r="B112">
+        <v>7</v>
+      </c>
+      <c r="C112" t="s">
+        <v>583</v>
+      </c>
+      <c r="D112">
+        <v>2</v>
+      </c>
+      <c r="E112">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="F112" t="s">
+        <v>584</v>
+      </c>
+      <c r="G112">
+        <v>150</v>
+      </c>
+      <c r="H112" t="s">
+        <v>585</v>
+      </c>
+      <c r="I112">
+        <v>7</v>
+      </c>
+      <c r="J112" t="s">
+        <v>586</v>
+      </c>
+      <c r="K112">
+        <v>360</v>
+      </c>
+      <c r="L112" t="s">
+        <v>587</v>
+      </c>
+      <c r="M112">
+        <v>40</v>
+      </c>
+      <c r="N112" t="s">
+        <v>511</v>
+      </c>
+      <c r="O112">
+        <v>363.33</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>589</v>
+      </c>
+      <c r="B113">
+        <v>7</v>
+      </c>
+      <c r="C113" t="s">
+        <v>590</v>
+      </c>
+      <c r="D113">
+        <v>2</v>
+      </c>
+      <c r="E113">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="F113" t="s">
+        <v>591</v>
+      </c>
+      <c r="G113">
+        <v>150</v>
+      </c>
+      <c r="H113" t="s">
+        <v>592</v>
+      </c>
+      <c r="I113">
+        <v>7</v>
+      </c>
+      <c r="J113" t="s">
+        <v>593</v>
+      </c>
+      <c r="K113">
+        <v>360</v>
+      </c>
+      <c r="L113" t="s">
+        <v>594</v>
+      </c>
+      <c r="M113">
+        <v>40</v>
+      </c>
+      <c r="N113" t="s">
+        <v>308</v>
+      </c>
+      <c r="O113">
+        <v>414.82</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>596</v>
+      </c>
+      <c r="B114">
+        <v>7</v>
+      </c>
+      <c r="C114" t="s">
+        <v>597</v>
+      </c>
+      <c r="D114">
+        <v>2</v>
+      </c>
+      <c r="E114">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="F114" t="s">
+        <v>598</v>
+      </c>
+      <c r="G114">
+        <v>150</v>
+      </c>
+      <c r="H114" t="s">
+        <v>599</v>
+      </c>
+      <c r="I114">
+        <v>7</v>
+      </c>
+      <c r="J114" t="s">
+        <v>600</v>
+      </c>
+      <c r="K114">
+        <v>360</v>
+      </c>
+      <c r="L114" t="s">
+        <v>601</v>
+      </c>
+      <c r="M114">
+        <v>40</v>
+      </c>
+      <c r="N114" t="s">
+        <v>665</v>
+      </c>
+      <c r="O114">
+        <v>19168.38</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>603</v>
+      </c>
+      <c r="B115">
+        <v>3</v>
+      </c>
+      <c r="C115" t="s">
+        <v>604</v>
+      </c>
+      <c r="D115">
+        <v>2</v>
+      </c>
+      <c r="E115">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F115" t="s">
+        <v>605</v>
+      </c>
+      <c r="G115">
+        <v>190</v>
+      </c>
+      <c r="H115" t="s">
+        <v>606</v>
+      </c>
+      <c r="I115">
+        <v>90</v>
+      </c>
+      <c r="J115" t="s">
+        <v>607</v>
+      </c>
+      <c r="K115">
+        <v>270</v>
+      </c>
+      <c r="L115" t="s">
+        <v>608</v>
+      </c>
+      <c r="M115">
+        <v>90</v>
+      </c>
+      <c r="N115" t="s">
+        <v>518</v>
+      </c>
+      <c r="O115">
+        <v>94.64</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>610</v>
+      </c>
+      <c r="B116">
+        <v>3</v>
+      </c>
+      <c r="C116" t="s">
+        <v>611</v>
+      </c>
+      <c r="D116">
+        <v>2</v>
+      </c>
+      <c r="E116">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F116" t="s">
+        <v>612</v>
+      </c>
+      <c r="G116">
+        <v>190</v>
+      </c>
+      <c r="H116" t="s">
+        <v>613</v>
+      </c>
+      <c r="I116">
+        <v>90</v>
+      </c>
+      <c r="J116" t="s">
+        <v>614</v>
+      </c>
+      <c r="K116">
+        <v>84</v>
+      </c>
+      <c r="L116" t="s">
+        <v>615</v>
+      </c>
+      <c r="M116">
+        <v>90</v>
+      </c>
+      <c r="N116" t="s">
+        <v>364</v>
+      </c>
+      <c r="O116">
+        <v>2399.61</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>617</v>
+      </c>
+      <c r="B117">
+        <v>3</v>
+      </c>
+      <c r="C117" t="s">
+        <v>618</v>
+      </c>
+      <c r="D117">
+        <v>2</v>
+      </c>
+      <c r="E117">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F117" t="s">
+        <v>619</v>
+      </c>
+      <c r="G117">
+        <v>190</v>
+      </c>
+      <c r="H117" t="s">
+        <v>620</v>
+      </c>
+      <c r="I117">
+        <v>90</v>
+      </c>
+      <c r="J117" t="s">
+        <v>621</v>
+      </c>
+      <c r="K117">
+        <v>84</v>
+      </c>
+      <c r="L117" t="s">
+        <v>622</v>
+      </c>
+      <c r="M117">
+        <v>90</v>
+      </c>
+      <c r="N117" t="s">
+        <v>672</v>
+      </c>
+      <c r="O117">
+        <v>1139292.8400000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>624</v>
+      </c>
+      <c r="B118">
+        <v>2</v>
+      </c>
+      <c r="C118" t="s">
+        <v>625</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F118" t="s">
+        <v>626</v>
+      </c>
+      <c r="G118">
+        <v>290</v>
+      </c>
+      <c r="H118" t="s">
+        <v>627</v>
+      </c>
+      <c r="I118">
+        <v>7</v>
+      </c>
+      <c r="J118" t="s">
+        <v>628</v>
+      </c>
+      <c r="K118">
+        <v>84</v>
+      </c>
+      <c r="L118" t="s">
+        <v>629</v>
+      </c>
+      <c r="M118">
+        <v>50</v>
+      </c>
+      <c r="N118" t="s">
+        <v>476</v>
+      </c>
+      <c r="O118">
+        <v>477.73</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>631</v>
+      </c>
+      <c r="B119">
+        <v>3</v>
+      </c>
+      <c r="C119" t="s">
+        <v>632</v>
+      </c>
+      <c r="D119">
+        <v>3</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="F119" t="s">
+        <v>633</v>
+      </c>
+      <c r="G119">
+        <v>230</v>
+      </c>
+      <c r="H119" t="s">
+        <v>634</v>
+      </c>
+      <c r="I119">
+        <v>7</v>
+      </c>
+      <c r="J119" t="s">
+        <v>635</v>
+      </c>
+      <c r="K119">
+        <v>330</v>
+      </c>
+      <c r="L119" t="s">
+        <v>636</v>
+      </c>
+      <c r="M119">
+        <v>30</v>
+      </c>
+      <c r="N119" t="s">
+        <v>287</v>
+      </c>
+      <c r="O119">
+        <v>98.32</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>638</v>
+      </c>
+      <c r="B120">
+        <v>8</v>
+      </c>
+      <c r="C120" t="s">
+        <v>639</v>
+      </c>
+      <c r="D120">
+        <v>2</v>
+      </c>
+      <c r="E120">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F120" t="s">
+        <v>640</v>
+      </c>
+      <c r="G120">
+        <v>270</v>
+      </c>
+      <c r="H120" t="s">
+        <v>641</v>
+      </c>
+      <c r="I120">
+        <v>7</v>
+      </c>
+      <c r="J120" t="s">
+        <v>642</v>
+      </c>
+      <c r="K120">
+        <v>360</v>
+      </c>
+      <c r="L120" t="s">
+        <v>643</v>
+      </c>
+      <c r="M120">
+        <v>60</v>
+      </c>
+      <c r="N120" t="s">
+        <v>315</v>
+      </c>
+      <c r="O120">
+        <v>213.49</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>645</v>
+      </c>
+      <c r="B121">
+        <v>9</v>
+      </c>
+      <c r="C121" t="s">
+        <v>646</v>
+      </c>
+      <c r="D121">
+        <v>3</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="F121" t="s">
+        <v>647</v>
+      </c>
+      <c r="G121">
+        <v>220</v>
+      </c>
+      <c r="H121" t="s">
+        <v>648</v>
+      </c>
+      <c r="I121">
+        <v>7</v>
+      </c>
+      <c r="J121" t="s">
+        <v>649</v>
+      </c>
+      <c r="K121">
+        <v>360</v>
+      </c>
+      <c r="L121" t="s">
+        <v>650</v>
+      </c>
+      <c r="M121">
+        <v>40</v>
+      </c>
+      <c r="N121" t="s">
+        <v>525</v>
+      </c>
+      <c r="O121">
+        <v>82.83</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>652</v>
+      </c>
+      <c r="B122">
+        <v>9</v>
+      </c>
+      <c r="C122" t="s">
+        <v>653</v>
+      </c>
+      <c r="D122">
+        <v>3</v>
+      </c>
+      <c r="E122">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="F122" t="s">
+        <v>654</v>
+      </c>
+      <c r="G122">
+        <v>220</v>
+      </c>
+      <c r="H122" t="s">
+        <v>655</v>
+      </c>
+      <c r="I122">
+        <v>7</v>
+      </c>
+      <c r="J122" t="s">
+        <v>656</v>
+      </c>
+      <c r="K122">
+        <v>360</v>
+      </c>
+      <c r="L122" t="s">
+        <v>657</v>
+      </c>
+      <c r="M122">
+        <v>40</v>
+      </c>
+      <c r="N122" t="s">
+        <v>301</v>
+      </c>
+      <c r="O122">
+        <v>38.090000000000003</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>659</v>
+      </c>
+      <c r="B123">
+        <v>7</v>
+      </c>
+      <c r="C123" t="s">
+        <v>660</v>
+      </c>
+      <c r="D123">
+        <v>3</v>
+      </c>
+      <c r="E123">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="F123" t="s">
+        <v>661</v>
+      </c>
+      <c r="G123">
+        <v>280</v>
+      </c>
+      <c r="H123" t="s">
+        <v>662</v>
+      </c>
+      <c r="I123">
+        <v>7</v>
+      </c>
+      <c r="J123" t="s">
+        <v>663</v>
+      </c>
+      <c r="K123">
+        <v>360</v>
+      </c>
+      <c r="L123" t="s">
+        <v>664</v>
+      </c>
+      <c r="M123">
+        <v>30</v>
+      </c>
+      <c r="N123" t="s">
+        <v>609</v>
+      </c>
+      <c r="O123">
+        <v>879.7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>666</v>
+      </c>
+      <c r="B124">
+        <v>7</v>
+      </c>
+      <c r="C124" t="s">
+        <v>667</v>
+      </c>
+      <c r="D124">
+        <v>3</v>
+      </c>
+      <c r="E124">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="F124" t="s">
+        <v>668</v>
+      </c>
+      <c r="G124">
+        <v>280</v>
+      </c>
+      <c r="H124" t="s">
+        <v>669</v>
+      </c>
+      <c r="I124">
+        <v>7</v>
+      </c>
+      <c r="J124" t="s">
+        <v>670</v>
+      </c>
+      <c r="K124">
+        <v>360</v>
+      </c>
+      <c r="L124" t="s">
+        <v>671</v>
+      </c>
+      <c r="M124">
+        <v>30</v>
+      </c>
+      <c r="N124" t="s">
+        <v>322</v>
+      </c>
+      <c r="O124">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>673</v>
+      </c>
+      <c r="B125">
+        <v>2</v>
+      </c>
+      <c r="C125" t="s">
+        <v>674</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+      <c r="E125">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F125" t="s">
+        <v>675</v>
+      </c>
+      <c r="G125">
+        <v>10</v>
+      </c>
+      <c r="H125" t="s">
+        <v>676</v>
+      </c>
+      <c r="I125">
+        <v>7</v>
+      </c>
+      <c r="J125" t="s">
+        <v>677</v>
+      </c>
+      <c r="K125">
+        <v>30</v>
+      </c>
+      <c r="L125" t="s">
+        <v>678</v>
+      </c>
+      <c r="M125">
+        <v>90</v>
+      </c>
+      <c r="N125" t="s">
+        <v>553</v>
+      </c>
+      <c r="O125">
+        <v>27.42</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F126" t="s">
+        <v>680</v>
+      </c>
+      <c r="G126">
+        <v>300</v>
+      </c>
+      <c r="H126" t="s">
+        <v>681</v>
+      </c>
+      <c r="I126">
+        <v>7</v>
+      </c>
+      <c r="J126" t="s">
+        <v>682</v>
+      </c>
+      <c r="K126">
+        <v>30</v>
+      </c>
+      <c r="L126" t="s">
+        <v>683</v>
+      </c>
+      <c r="M126">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F127" t="s">
+        <v>684</v>
+      </c>
+      <c r="G127">
+        <v>300</v>
+      </c>
+      <c r="H127" t="s">
+        <v>685</v>
+      </c>
+      <c r="I127">
+        <v>7</v>
+      </c>
+      <c r="J127" t="s">
+        <v>686</v>
+      </c>
+      <c r="K127">
+        <v>30</v>
+      </c>
+      <c r="L127" t="s">
+        <v>687</v>
+      </c>
+      <c r="M127">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F128" t="s">
+        <v>688</v>
+      </c>
+      <c r="G128">
+        <v>300</v>
+      </c>
+      <c r="H128" t="s">
+        <v>689</v>
+      </c>
+      <c r="I128">
+        <v>7</v>
+      </c>
+      <c r="J128" t="s">
+        <v>690</v>
+      </c>
+      <c r="K128">
+        <v>30</v>
+      </c>
+      <c r="L128" t="s">
+        <v>691</v>
+      </c>
+      <c r="M128">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="129" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F129" t="s">
+        <v>692</v>
+      </c>
+      <c r="G129">
+        <v>300</v>
+      </c>
+      <c r="H129" t="s">
+        <v>693</v>
+      </c>
+      <c r="I129">
+        <v>7</v>
+      </c>
+      <c r="J129" t="s">
+        <v>694</v>
+      </c>
+      <c r="K129">
+        <v>30</v>
+      </c>
+      <c r="L129" t="s">
+        <v>695</v>
+      </c>
+      <c r="M129">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="R1:R1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>370</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10277,8 +13255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q131"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="G9" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13843,6 +16821,16 @@
     <sortCondition ref="R1:R118"/>
     <sortCondition ref="S1:S118"/>
   </sortState>
+  <conditionalFormatting sqref="Q1:Q1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update recruit spreadsheet, looking for error in timing
</commit_message>
<xml_diff>
--- a/R/BHrecruits.xlsx
+++ b/R/BHrecruits.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan.morse\Documents\GitHub\atneus_RM\R\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="554" activeTab="1"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="spawn" sheetId="2" r:id="rId2"/>
     <sheet name="mig" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -3277,7 +3272,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
@@ -3290,12 +3285,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3310,16 +3311,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3416,7 +3438,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3451,7 +3473,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6822,8 +6844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="Q79" sqref="Q79"/>
+    <sheetView tabSelected="1" topLeftCell="D56" workbookViewId="0">
+      <selection activeCell="S68" sqref="S68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10340,53 +10362,77 @@
       <c r="O67">
         <v>1.1599999999999999</v>
       </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="Q67">
+        <f>G67+K67</f>
+        <v>240</v>
+      </c>
+      <c r="R67">
+        <f>Q67+I67</f>
+        <v>247</v>
+      </c>
+      <c r="S67">
+        <f>R67+M67</f>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="B68" s="4">
+        <v>1</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="4">
         <v>2</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="4">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="G68">
+      <c r="G68" s="4">
         <v>290</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H68" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="I68">
+      <c r="I68" s="4">
         <v>7</v>
       </c>
-      <c r="J68" t="s">
+      <c r="J68" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="K68">
+      <c r="K68" s="4">
         <v>30</v>
       </c>
-      <c r="L68" t="s">
+      <c r="L68" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="M68">
+      <c r="M68" s="4">
         <v>60</v>
       </c>
-      <c r="N68" t="s">
+      <c r="N68" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="O68">
+      <c r="O68" s="4">
         <v>27900.25</v>
+      </c>
+      <c r="Q68" s="4">
+        <f t="shared" ref="Q68:Q125" si="5">G68+K68</f>
+        <v>320</v>
+      </c>
+      <c r="R68" s="4">
+        <f t="shared" ref="R68:R78" si="6">Q68+I68</f>
+        <v>327</v>
+      </c>
+      <c r="S68" s="4">
+        <f t="shared" ref="S68:S125" si="7">R68+M68</f>
+        <v>387</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
@@ -10436,6 +10482,18 @@
       <c r="O69">
         <v>21083.35</v>
       </c>
+      <c r="Q69">
+        <f t="shared" si="5"/>
+        <v>240</v>
+      </c>
+      <c r="R69">
+        <f t="shared" si="6"/>
+        <v>247</v>
+      </c>
+      <c r="S69">
+        <f t="shared" si="7"/>
+        <v>337</v>
+      </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
@@ -10484,6 +10542,18 @@
       <c r="O70">
         <v>99.5</v>
       </c>
+      <c r="Q70">
+        <f t="shared" si="5"/>
+        <v>210</v>
+      </c>
+      <c r="R70">
+        <f t="shared" si="6"/>
+        <v>217</v>
+      </c>
+      <c r="S70">
+        <f t="shared" si="7"/>
+        <v>247</v>
+      </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -10532,6 +10602,18 @@
       <c r="O71">
         <v>5678.88</v>
       </c>
+      <c r="Q71">
+        <f t="shared" si="5"/>
+        <v>260</v>
+      </c>
+      <c r="R71">
+        <f t="shared" si="6"/>
+        <v>267</v>
+      </c>
+      <c r="S71">
+        <f t="shared" si="7"/>
+        <v>357</v>
+      </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
@@ -10580,6 +10662,18 @@
       <c r="O72">
         <v>17.809999999999999</v>
       </c>
+      <c r="Q72">
+        <f t="shared" si="5"/>
+        <v>350</v>
+      </c>
+      <c r="R72">
+        <f t="shared" si="6"/>
+        <v>357</v>
+      </c>
+      <c r="S72">
+        <f t="shared" si="7"/>
+        <v>447</v>
+      </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
@@ -10628,6 +10722,18 @@
       <c r="O73">
         <v>134.86000000000001</v>
       </c>
+      <c r="Q73">
+        <f t="shared" si="5"/>
+        <v>110</v>
+      </c>
+      <c r="R73">
+        <f t="shared" si="6"/>
+        <v>117</v>
+      </c>
+      <c r="S73">
+        <f t="shared" si="7"/>
+        <v>207</v>
+      </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
@@ -10676,6 +10782,18 @@
       <c r="O74">
         <v>11.95</v>
       </c>
+      <c r="Q74">
+        <f t="shared" si="5"/>
+        <v>220</v>
+      </c>
+      <c r="R74">
+        <f t="shared" si="6"/>
+        <v>227</v>
+      </c>
+      <c r="S74">
+        <f t="shared" si="7"/>
+        <v>317</v>
+      </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
@@ -10724,6 +10842,18 @@
       <c r="O75">
         <v>3525480.78</v>
       </c>
+      <c r="Q75">
+        <f t="shared" si="5"/>
+        <v>260</v>
+      </c>
+      <c r="R75">
+        <f t="shared" si="6"/>
+        <v>267</v>
+      </c>
+      <c r="S75">
+        <f t="shared" si="7"/>
+        <v>357</v>
+      </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
@@ -10772,6 +10902,18 @@
       <c r="O76">
         <v>763.46</v>
       </c>
+      <c r="Q76">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
+      <c r="R76">
+        <f t="shared" si="6"/>
+        <v>187</v>
+      </c>
+      <c r="S76">
+        <f t="shared" si="7"/>
+        <v>277</v>
+      </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
@@ -10820,6 +10962,18 @@
       <c r="O77">
         <v>795.66</v>
       </c>
+      <c r="Q77">
+        <f t="shared" si="5"/>
+        <v>260</v>
+      </c>
+      <c r="R77">
+        <f t="shared" si="6"/>
+        <v>267</v>
+      </c>
+      <c r="S77">
+        <f t="shared" si="7"/>
+        <v>357</v>
+      </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
@@ -10868,164 +11022,200 @@
       <c r="O78">
         <v>95.78</v>
       </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="Q78">
+        <f t="shared" si="5"/>
+        <v>260</v>
+      </c>
+      <c r="R78">
+        <f t="shared" si="6"/>
+        <v>267</v>
+      </c>
+      <c r="S78">
+        <f t="shared" si="7"/>
+        <v>357</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="4">
         <v>3</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="4">
         <v>3</v>
       </c>
-      <c r="E79">
+      <c r="E79" s="4">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="G79">
+      <c r="G79" s="4">
         <v>180</v>
       </c>
-      <c r="H79" t="s">
+      <c r="H79" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="I79">
+      <c r="I79" s="4">
         <v>7</v>
       </c>
-      <c r="J79" t="s">
+      <c r="J79" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="K79">
+      <c r="K79" s="4">
         <v>180</v>
       </c>
-      <c r="L79" t="s">
+      <c r="L79" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="M79">
+      <c r="M79" s="4">
         <v>60</v>
       </c>
-      <c r="N79" t="s">
+      <c r="N79" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="O79">
+      <c r="O79" s="4">
         <v>21317.17</v>
       </c>
-      <c r="Q79">
-        <f>G79+K79+I79</f>
+      <c r="Q79" s="4">
+        <f t="shared" si="5"/>
+        <v>360</v>
+      </c>
+      <c r="R79" s="4">
+        <f>Q79+I79</f>
         <v>367</v>
       </c>
-      <c r="R79">
-        <f>Q79+M79</f>
+      <c r="S79" s="4">
+        <f t="shared" si="7"/>
         <v>427</v>
       </c>
-      <c r="S79">
-        <f>R79-365-I79</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    </row>
+    <row r="80" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="4">
         <v>3</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="4">
         <v>3</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="4">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="G80">
+      <c r="G80" s="4">
         <v>180</v>
       </c>
-      <c r="H80" t="s">
+      <c r="H80" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="I80">
+      <c r="I80" s="4">
         <v>7</v>
       </c>
-      <c r="J80" t="s">
+      <c r="J80" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="K80">
+      <c r="K80" s="4">
         <v>180</v>
       </c>
-      <c r="L80" t="s">
+      <c r="L80" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="M80">
+      <c r="M80" s="4">
         <v>60</v>
       </c>
-      <c r="N80" t="s">
+      <c r="N80" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="O80">
+      <c r="O80" s="4">
         <v>82.43</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="Q80" s="4">
+        <f t="shared" si="5"/>
+        <v>360</v>
+      </c>
+      <c r="R80" s="4">
+        <f t="shared" ref="R80:R125" si="8">Q80+I80</f>
+        <v>367</v>
+      </c>
+      <c r="S80" s="4">
+        <f t="shared" si="7"/>
+        <v>427</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="4">
         <v>3</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="4">
         <v>3</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="4">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="G81">
+      <c r="G81" s="4">
         <v>180</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H81" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="I81">
+      <c r="I81" s="4">
         <v>7</v>
       </c>
-      <c r="J81" t="s">
+      <c r="J81" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="K81">
+      <c r="K81" s="4">
         <v>180</v>
       </c>
-      <c r="L81" t="s">
+      <c r="L81" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="M81">
+      <c r="M81" s="4">
         <v>60</v>
       </c>
-      <c r="N81" t="s">
+      <c r="N81" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="O81">
+      <c r="O81" s="4">
         <v>54.03</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q81" s="4">
+        <f t="shared" si="5"/>
+        <v>360</v>
+      </c>
+      <c r="R81" s="4">
+        <f t="shared" si="8"/>
+        <v>367</v>
+      </c>
+      <c r="S81" s="4">
+        <f t="shared" si="7"/>
+        <v>427</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>372</v>
       </c>
@@ -11072,8 +11262,20 @@
       <c r="O82">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q82">
+        <f t="shared" si="5"/>
+        <v>205</v>
+      </c>
+      <c r="R82">
+        <f t="shared" si="8"/>
+        <v>212</v>
+      </c>
+      <c r="S82">
+        <f t="shared" si="7"/>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>379</v>
       </c>
@@ -11120,8 +11322,20 @@
       <c r="O83">
         <v>24.13</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q83">
+        <f t="shared" si="5"/>
+        <v>135</v>
+      </c>
+      <c r="R83">
+        <f t="shared" si="8"/>
+        <v>142</v>
+      </c>
+      <c r="S83">
+        <f t="shared" si="7"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>386</v>
       </c>
@@ -11168,8 +11382,20 @@
       <c r="O84">
         <v>154.37</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q84">
+        <f t="shared" si="5"/>
+        <v>135</v>
+      </c>
+      <c r="R84">
+        <f t="shared" si="8"/>
+        <v>142</v>
+      </c>
+      <c r="S84">
+        <f t="shared" si="7"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>393</v>
       </c>
@@ -11216,56 +11442,80 @@
       <c r="O85">
         <v>143.11000000000001</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="Q85">
+        <f t="shared" si="5"/>
+        <v>135</v>
+      </c>
+      <c r="R85">
+        <f t="shared" si="8"/>
+        <v>142</v>
+      </c>
+      <c r="S85">
+        <f t="shared" si="7"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="B86">
-        <v>1</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="B86" s="4">
+        <v>1</v>
+      </c>
+      <c r="C86" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="4">
         <v>3</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="4">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="G86">
+      <c r="G86" s="4">
         <v>280</v>
       </c>
-      <c r="H86" t="s">
+      <c r="H86" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="I86">
+      <c r="I86" s="4">
         <v>7</v>
       </c>
-      <c r="J86" t="s">
+      <c r="J86" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="K86">
+      <c r="K86" s="4">
         <v>60</v>
       </c>
-      <c r="L86" t="s">
+      <c r="L86" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="M86">
+      <c r="M86" s="4">
         <v>60</v>
       </c>
-      <c r="N86" t="s">
+      <c r="N86" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="O86">
+      <c r="O86" s="4">
         <v>3825.02</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q86" s="4">
+        <f t="shared" si="5"/>
+        <v>340</v>
+      </c>
+      <c r="R86" s="4">
+        <f t="shared" si="8"/>
+        <v>347</v>
+      </c>
+      <c r="S86" s="4">
+        <f t="shared" si="7"/>
+        <v>407</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>407</v>
       </c>
@@ -11312,8 +11562,20 @@
       <c r="O87">
         <v>13.34</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q87">
+        <f t="shared" si="5"/>
+        <v>300</v>
+      </c>
+      <c r="R87">
+        <f t="shared" si="8"/>
+        <v>307</v>
+      </c>
+      <c r="S87">
+        <f t="shared" si="7"/>
+        <v>347</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>414</v>
       </c>
@@ -11360,8 +11622,20 @@
       <c r="O88">
         <v>82.92</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q88">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="R88">
+        <f t="shared" si="8"/>
+        <v>47</v>
+      </c>
+      <c r="S88">
+        <f t="shared" si="7"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>421</v>
       </c>
@@ -11408,8 +11682,20 @@
       <c r="O89">
         <v>207.63</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q89">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="R89">
+        <f t="shared" si="8"/>
+        <v>87</v>
+      </c>
+      <c r="S89">
+        <f t="shared" si="7"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>428</v>
       </c>
@@ -11456,8 +11742,20 @@
       <c r="O90">
         <v>18.11</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q90">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
+      <c r="R90">
+        <f t="shared" si="8"/>
+        <v>187</v>
+      </c>
+      <c r="S90">
+        <f t="shared" si="7"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>435</v>
       </c>
@@ -11504,8 +11802,20 @@
       <c r="O91">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q91">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
+      <c r="R91">
+        <f t="shared" si="8"/>
+        <v>187</v>
+      </c>
+      <c r="S91">
+        <f t="shared" si="7"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>442</v>
       </c>
@@ -11552,8 +11862,20 @@
       <c r="O92">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q92">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="R92">
+        <f t="shared" si="8"/>
+        <v>47</v>
+      </c>
+      <c r="S92">
+        <f t="shared" si="7"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>449</v>
       </c>
@@ -11600,8 +11922,20 @@
       <c r="O93">
         <v>32.65</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q93">
+        <f t="shared" si="5"/>
+        <v>210</v>
+      </c>
+      <c r="R93">
+        <f t="shared" si="8"/>
+        <v>217</v>
+      </c>
+      <c r="S93">
+        <f t="shared" si="7"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>456</v>
       </c>
@@ -11648,8 +11982,20 @@
       <c r="O94">
         <v>127.1</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q94">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
+      <c r="R94">
+        <f t="shared" si="8"/>
+        <v>187</v>
+      </c>
+      <c r="S94">
+        <f t="shared" si="7"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>463</v>
       </c>
@@ -11696,8 +12042,20 @@
       <c r="O95">
         <v>11810.41</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q95">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
+      <c r="R95">
+        <f t="shared" si="8"/>
+        <v>187</v>
+      </c>
+      <c r="S95">
+        <f t="shared" si="7"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>470</v>
       </c>
@@ -11744,8 +12102,20 @@
       <c r="O96">
         <v>77.02</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q96">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
+      <c r="R96">
+        <f t="shared" si="8"/>
+        <v>187</v>
+      </c>
+      <c r="S96">
+        <f t="shared" si="7"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>477</v>
       </c>
@@ -11792,8 +12162,20 @@
       <c r="O97">
         <v>621.19000000000005</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q97">
+        <f t="shared" si="5"/>
+        <v>130</v>
+      </c>
+      <c r="R97">
+        <f t="shared" si="8"/>
+        <v>137</v>
+      </c>
+      <c r="S97">
+        <f t="shared" si="7"/>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>484</v>
       </c>
@@ -11840,8 +12222,20 @@
       <c r="O98">
         <v>7165.5</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q98">
+        <f t="shared" si="5"/>
+        <v>130</v>
+      </c>
+      <c r="R98">
+        <f t="shared" si="8"/>
+        <v>137</v>
+      </c>
+      <c r="S98">
+        <f t="shared" si="7"/>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>491</v>
       </c>
@@ -11888,8 +12282,20 @@
       <c r="O99">
         <v>21158.53</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q99">
+        <f t="shared" si="5"/>
+        <v>250</v>
+      </c>
+      <c r="R99">
+        <f t="shared" si="8"/>
+        <v>257</v>
+      </c>
+      <c r="S99">
+        <f t="shared" si="7"/>
+        <v>347</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>498</v>
       </c>
@@ -11936,8 +12342,20 @@
       <c r="O100">
         <v>8.73</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q100">
+        <f t="shared" si="5"/>
+        <v>210</v>
+      </c>
+      <c r="R100">
+        <f t="shared" si="8"/>
+        <v>217</v>
+      </c>
+      <c r="S100">
+        <f t="shared" si="7"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>505</v>
       </c>
@@ -11984,8 +12402,20 @@
       <c r="O101">
         <v>12248.15</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q101">
+        <f t="shared" si="5"/>
+        <v>210</v>
+      </c>
+      <c r="R101">
+        <f t="shared" si="8"/>
+        <v>217</v>
+      </c>
+      <c r="S101">
+        <f t="shared" si="7"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>512</v>
       </c>
@@ -12032,8 +12462,20 @@
       <c r="O102">
         <v>111.1</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q102">
+        <f t="shared" si="5"/>
+        <v>210</v>
+      </c>
+      <c r="R102">
+        <f t="shared" si="8"/>
+        <v>217</v>
+      </c>
+      <c r="S102">
+        <f t="shared" si="7"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>519</v>
       </c>
@@ -12080,8 +12522,20 @@
       <c r="O103">
         <v>4310573.47</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q103">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="R103">
+        <f t="shared" si="8"/>
+        <v>47</v>
+      </c>
+      <c r="S103">
+        <f t="shared" si="7"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>526</v>
       </c>
@@ -12128,8 +12582,20 @@
       <c r="O104">
         <v>1035.6400000000001</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q104">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="R104">
+        <f t="shared" si="8"/>
+        <v>47</v>
+      </c>
+      <c r="S104">
+        <f t="shared" si="7"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>533</v>
       </c>
@@ -12176,8 +12642,20 @@
       <c r="O105">
         <v>54.32</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q105">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="R105">
+        <f t="shared" si="8"/>
+        <v>47</v>
+      </c>
+      <c r="S105">
+        <f t="shared" si="7"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>540</v>
       </c>
@@ -12224,8 +12702,20 @@
       <c r="O106">
         <v>56.67</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q106">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="R106">
+        <f t="shared" si="8"/>
+        <v>67</v>
+      </c>
+      <c r="S106">
+        <f t="shared" si="7"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>547</v>
       </c>
@@ -12272,56 +12762,80 @@
       <c r="O107">
         <v>476.74</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="Q107">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="R107">
+        <f t="shared" si="8"/>
+        <v>107</v>
+      </c>
+      <c r="S107">
+        <f t="shared" si="7"/>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="4">
         <v>4</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="D108">
+      <c r="D108" s="4">
         <v>3</v>
       </c>
-      <c r="E108">
+      <c r="E108" s="4">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="F108" t="s">
+      <c r="F108" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="G108">
+      <c r="G108" s="4">
         <v>180</v>
       </c>
-      <c r="H108" t="s">
+      <c r="H108" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="I108">
+      <c r="I108" s="4">
         <v>7</v>
       </c>
-      <c r="J108" t="s">
+      <c r="J108" s="4" t="s">
         <v>558</v>
       </c>
-      <c r="K108">
+      <c r="K108" s="4">
         <v>270</v>
       </c>
-      <c r="L108" t="s">
+      <c r="L108" s="4" t="s">
         <v>559</v>
       </c>
-      <c r="M108">
+      <c r="M108" s="4">
         <v>90</v>
       </c>
-      <c r="N108" t="s">
+      <c r="N108" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="O108">
+      <c r="O108" s="4">
         <v>23.28</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q108" s="4">
+        <f t="shared" si="5"/>
+        <v>450</v>
+      </c>
+      <c r="R108" s="4">
+        <f t="shared" si="8"/>
+        <v>457</v>
+      </c>
+      <c r="S108" s="4">
+        <f t="shared" si="7"/>
+        <v>547</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>561</v>
       </c>
@@ -12368,8 +12882,20 @@
       <c r="O109">
         <v>1201.82</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q109">
+        <f t="shared" si="5"/>
+        <v>520</v>
+      </c>
+      <c r="R109">
+        <f t="shared" si="8"/>
+        <v>527</v>
+      </c>
+      <c r="S109">
+        <f t="shared" si="7"/>
+        <v>617</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>568</v>
       </c>
@@ -12416,8 +12942,20 @@
       <c r="O110">
         <v>436.41</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q110">
+        <f t="shared" si="5"/>
+        <v>520</v>
+      </c>
+      <c r="R110">
+        <f t="shared" si="8"/>
+        <v>527</v>
+      </c>
+      <c r="S110">
+        <f t="shared" si="7"/>
+        <v>617</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>575</v>
       </c>
@@ -12464,8 +13002,20 @@
       <c r="O111">
         <v>3884.39</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q111">
+        <f t="shared" si="5"/>
+        <v>520</v>
+      </c>
+      <c r="R111">
+        <f t="shared" si="8"/>
+        <v>527</v>
+      </c>
+      <c r="S111">
+        <f t="shared" si="7"/>
+        <v>617</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>582</v>
       </c>
@@ -12512,8 +13062,20 @@
       <c r="O112">
         <v>363.33</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q112">
+        <f t="shared" si="5"/>
+        <v>510</v>
+      </c>
+      <c r="R112">
+        <f t="shared" si="8"/>
+        <v>517</v>
+      </c>
+      <c r="S112">
+        <f t="shared" si="7"/>
+        <v>557</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>589</v>
       </c>
@@ -12560,8 +13122,20 @@
       <c r="O113">
         <v>414.82</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q113">
+        <f t="shared" si="5"/>
+        <v>510</v>
+      </c>
+      <c r="R113">
+        <f t="shared" si="8"/>
+        <v>517</v>
+      </c>
+      <c r="S113">
+        <f t="shared" si="7"/>
+        <v>557</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>596</v>
       </c>
@@ -12608,248 +13182,320 @@
       <c r="O114">
         <v>19168.38</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="Q114">
+        <f t="shared" si="5"/>
+        <v>510</v>
+      </c>
+      <c r="R114">
+        <f t="shared" si="8"/>
+        <v>517</v>
+      </c>
+      <c r="S114">
+        <f t="shared" si="7"/>
+        <v>557</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
         <v>603</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="4">
         <v>3</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="D115">
+      <c r="D115" s="4">
         <v>2</v>
       </c>
-      <c r="E115">
+      <c r="E115" s="4">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="F115" t="s">
+      <c r="F115" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="G115">
+      <c r="G115" s="4">
         <v>190</v>
       </c>
-      <c r="H115" t="s">
+      <c r="H115" s="4" t="s">
         <v>606</v>
       </c>
-      <c r="I115">
+      <c r="I115" s="4">
         <v>90</v>
       </c>
-      <c r="J115" t="s">
+      <c r="J115" s="4" t="s">
         <v>607</v>
       </c>
-      <c r="K115">
+      <c r="K115" s="4">
         <v>270</v>
       </c>
-      <c r="L115" t="s">
+      <c r="L115" s="4" t="s">
         <v>608</v>
       </c>
-      <c r="M115">
+      <c r="M115" s="4">
         <v>90</v>
       </c>
-      <c r="N115" t="s">
+      <c r="N115" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="O115">
+      <c r="O115" s="4">
         <v>94.64</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="Q115" s="4">
+        <f t="shared" si="5"/>
+        <v>460</v>
+      </c>
+      <c r="R115" s="4">
+        <f t="shared" si="8"/>
+        <v>550</v>
+      </c>
+      <c r="S115" s="4">
+        <f t="shared" si="7"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
         <v>610</v>
       </c>
-      <c r="B116">
+      <c r="B116" s="4">
         <v>3</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="4" t="s">
         <v>611</v>
       </c>
-      <c r="D116">
+      <c r="D116" s="4">
         <v>2</v>
       </c>
-      <c r="E116">
+      <c r="E116" s="4">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="F116" t="s">
+      <c r="F116" s="4" t="s">
         <v>612</v>
       </c>
-      <c r="G116">
+      <c r="G116" s="4">
         <v>190</v>
       </c>
-      <c r="H116" t="s">
+      <c r="H116" s="4" t="s">
         <v>613</v>
       </c>
-      <c r="I116">
+      <c r="I116" s="4">
         <v>90</v>
       </c>
-      <c r="J116" t="s">
+      <c r="J116" s="4" t="s">
         <v>614</v>
       </c>
-      <c r="K116">
+      <c r="K116" s="4">
         <v>84</v>
       </c>
-      <c r="L116" t="s">
+      <c r="L116" s="4" t="s">
         <v>615</v>
       </c>
-      <c r="M116">
+      <c r="M116" s="4">
         <v>90</v>
       </c>
-      <c r="N116" t="s">
+      <c r="N116" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="O116">
+      <c r="O116" s="4">
         <v>2399.61</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="Q116" s="4">
+        <f t="shared" si="5"/>
+        <v>274</v>
+      </c>
+      <c r="R116" s="4">
+        <f t="shared" si="8"/>
+        <v>364</v>
+      </c>
+      <c r="S116" s="4">
+        <f t="shared" si="7"/>
+        <v>454</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
         <v>617</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="4">
         <v>3</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="4" t="s">
         <v>618</v>
       </c>
-      <c r="D117">
+      <c r="D117" s="4">
         <v>2</v>
       </c>
-      <c r="E117">
+      <c r="E117" s="4">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="F117" t="s">
+      <c r="F117" s="4" t="s">
         <v>619</v>
       </c>
-      <c r="G117">
+      <c r="G117" s="4">
         <v>190</v>
       </c>
-      <c r="H117" t="s">
+      <c r="H117" s="4" t="s">
         <v>620</v>
       </c>
-      <c r="I117">
+      <c r="I117" s="4">
         <v>90</v>
       </c>
-      <c r="J117" t="s">
+      <c r="J117" s="4" t="s">
         <v>621</v>
       </c>
-      <c r="K117">
+      <c r="K117" s="4">
         <v>84</v>
       </c>
-      <c r="L117" t="s">
+      <c r="L117" s="4" t="s">
         <v>622</v>
       </c>
-      <c r="M117">
+      <c r="M117" s="4">
         <v>90</v>
       </c>
-      <c r="N117" t="s">
+      <c r="N117" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="O117">
+      <c r="O117" s="4">
         <v>1139292.8400000001</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="Q117" s="4">
+        <f t="shared" si="5"/>
+        <v>274</v>
+      </c>
+      <c r="R117" s="4">
+        <f t="shared" si="8"/>
+        <v>364</v>
+      </c>
+      <c r="S117" s="4">
+        <f t="shared" si="7"/>
+        <v>454</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="4">
         <v>2</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" s="4" t="s">
         <v>625</v>
       </c>
-      <c r="D118">
-        <v>1</v>
-      </c>
-      <c r="E118">
+      <c r="D118" s="4">
+        <v>1</v>
+      </c>
+      <c r="E118" s="4">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="F118" t="s">
+      <c r="F118" s="4" t="s">
         <v>626</v>
       </c>
-      <c r="G118">
+      <c r="G118" s="4">
         <v>290</v>
       </c>
-      <c r="H118" t="s">
+      <c r="H118" s="4" t="s">
         <v>627</v>
       </c>
-      <c r="I118">
+      <c r="I118" s="4">
         <v>7</v>
       </c>
-      <c r="J118" t="s">
+      <c r="J118" s="4" t="s">
         <v>628</v>
       </c>
-      <c r="K118">
+      <c r="K118" s="4">
         <v>84</v>
       </c>
-      <c r="L118" t="s">
+      <c r="L118" s="4" t="s">
         <v>629</v>
       </c>
-      <c r="M118">
+      <c r="M118" s="4">
         <v>50</v>
       </c>
-      <c r="N118" t="s">
+      <c r="N118" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="O118">
+      <c r="O118" s="4">
         <v>477.73</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="Q118" s="4">
+        <f t="shared" si="5"/>
+        <v>374</v>
+      </c>
+      <c r="R118" s="4">
+        <f t="shared" si="8"/>
+        <v>381</v>
+      </c>
+      <c r="S118" s="4">
+        <f t="shared" si="7"/>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="4">
         <v>3</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="4" t="s">
         <v>632</v>
       </c>
-      <c r="D119">
+      <c r="D119" s="4">
         <v>3</v>
       </c>
-      <c r="E119">
+      <c r="E119" s="4">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="F119" t="s">
+      <c r="F119" s="4" t="s">
         <v>633</v>
       </c>
-      <c r="G119">
+      <c r="G119" s="4">
         <v>230</v>
       </c>
-      <c r="H119" t="s">
+      <c r="H119" s="4" t="s">
         <v>634</v>
       </c>
-      <c r="I119">
+      <c r="I119" s="4">
         <v>7</v>
       </c>
-      <c r="J119" t="s">
+      <c r="J119" s="4" t="s">
         <v>635</v>
       </c>
-      <c r="K119">
+      <c r="K119" s="4">
         <v>330</v>
       </c>
-      <c r="L119" t="s">
+      <c r="L119" s="4" t="s">
         <v>636</v>
       </c>
-      <c r="M119">
+      <c r="M119" s="4">
         <v>30</v>
       </c>
-      <c r="N119" t="s">
+      <c r="N119" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="O119">
+      <c r="O119" s="4">
         <v>98.32</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q119" s="4">
+        <f t="shared" si="5"/>
+        <v>560</v>
+      </c>
+      <c r="R119" s="4">
+        <f t="shared" si="8"/>
+        <v>567</v>
+      </c>
+      <c r="S119" s="4">
+        <f t="shared" si="7"/>
+        <v>597</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>638</v>
       </c>
@@ -12896,8 +13542,20 @@
       <c r="O120">
         <v>213.49</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q120">
+        <f t="shared" si="5"/>
+        <v>630</v>
+      </c>
+      <c r="R120">
+        <f t="shared" si="8"/>
+        <v>637</v>
+      </c>
+      <c r="S120">
+        <f t="shared" si="7"/>
+        <v>697</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>645</v>
       </c>
@@ -12944,8 +13602,20 @@
       <c r="O121">
         <v>82.83</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q121">
+        <f t="shared" si="5"/>
+        <v>580</v>
+      </c>
+      <c r="R121">
+        <f t="shared" si="8"/>
+        <v>587</v>
+      </c>
+      <c r="S121">
+        <f t="shared" si="7"/>
+        <v>627</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>652</v>
       </c>
@@ -12992,8 +13662,20 @@
       <c r="O122">
         <v>38.090000000000003</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q122">
+        <f t="shared" si="5"/>
+        <v>580</v>
+      </c>
+      <c r="R122">
+        <f t="shared" si="8"/>
+        <v>587</v>
+      </c>
+      <c r="S122">
+        <f t="shared" si="7"/>
+        <v>627</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>659</v>
       </c>
@@ -13040,8 +13722,20 @@
       <c r="O123">
         <v>879.7</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q123">
+        <f t="shared" si="5"/>
+        <v>640</v>
+      </c>
+      <c r="R123">
+        <f t="shared" si="8"/>
+        <v>647</v>
+      </c>
+      <c r="S123">
+        <f t="shared" si="7"/>
+        <v>677</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>666</v>
       </c>
@@ -13088,8 +13782,20 @@
       <c r="O124">
         <v>42</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q124">
+        <f t="shared" si="5"/>
+        <v>640</v>
+      </c>
+      <c r="R124">
+        <f t="shared" si="8"/>
+        <v>647</v>
+      </c>
+      <c r="S124">
+        <f t="shared" si="7"/>
+        <v>677</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>673</v>
       </c>
@@ -13136,8 +13842,20 @@
       <c r="O125">
         <v>27.42</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q125">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="R125">
+        <f t="shared" si="8"/>
+        <v>47</v>
+      </c>
+      <c r="S125">
+        <f t="shared" si="7"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F126" t="s">
         <v>680</v>
       </c>
@@ -13163,7 +13881,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F127" t="s">
         <v>684</v>
       </c>
@@ -13189,7 +13907,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F128" t="s">
         <v>688</v>
       </c>
@@ -13243,7 +13961,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="R1:R1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>370</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16822,12 +17540,12 @@
     <sortCondition ref="S1:S118"/>
   </sortState>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
working on periodicity issue with output time, update fishbase pulls
</commit_message>
<xml_diff>
--- a/R/BHrecruits.xlsx
+++ b/R/BHrecruits.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan.morse\Documents\GitHub\atneus_RM\R\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="554" activeTab="1"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="spawn" sheetId="2" r:id="rId2"/>
     <sheet name="mig" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -3272,7 +3277,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
@@ -3321,37 +3326,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3438,7 +3413,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3473,7 +3448,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6844,8 +6819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D56" workbookViewId="0">
-      <selection activeCell="S68" sqref="S68"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13961,7 +13936,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="R1:R1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>370</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13973,8 +13948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q131"/>
   <sheetViews>
-    <sheetView topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="G9" sqref="G1:G1048576"/>
+    <sheetView topLeftCell="B85" workbookViewId="0">
+      <selection activeCell="Q40" sqref="Q40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17540,12 +17515,12 @@
     <sortCondition ref="S1:S118"/>
   </sortState>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>